<commit_message>
WPG SFRA 6.0 release
</commit_message>
<xml_diff>
--- a/test/testData/Worldpay_TestData.xlsx
+++ b/test/testData/Worldpay_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanraich\Documents\New_TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WPG_Automation_Release\sapient-project-worldpay-sfcc\test\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="203">
   <si>
     <t>Test card numbers</t>
   </si>
@@ -616,9 +616,6 @@
     <t>Russia</t>
   </si>
   <si>
-    <t>Klarna</t>
-  </si>
-  <si>
     <t>US,ALL</t>
   </si>
   <si>
@@ -637,68 +634,23 @@
     <t>APMs TEST DATA</t>
   </si>
   <si>
-    <t>Successful Frictionless Authentication</t>
-  </si>
-  <si>
-    <t>Magic Value</t>
-  </si>
-  <si>
-    <t>Overview</t>
-  </si>
-  <si>
-    <t>Response Data</t>
-  </si>
-  <si>
-    <t>EE_3DS.HONOURED_ISSUER_HONOURED.AUTHORISED</t>
-  </si>
-  <si>
-    <t>lastEvent = AUTHORISED</t>
-  </si>
-  <si>
-    <t>result = HONOURED</t>
-  </si>
-  <si>
-    <t>reason = ISSUER_HONOURED</t>
-  </si>
-  <si>
-    <t>3SD2 Frictionless Authentication Unavailable</t>
-  </si>
-  <si>
-    <t>EE_3DS_SCA.REJECTED_HIGH_RISK.AUTHORISED</t>
-  </si>
-  <si>
-    <t>Challenge required</t>
-  </si>
-  <si>
-    <t>result = REJECTED</t>
-  </si>
-  <si>
-    <t>reason = HIGH_RISK</t>
-  </si>
-  <si>
-    <t>EE_3DS_SCA.REJECTED_ISSUER_REJECTED.AUTHORISED</t>
-  </si>
-  <si>
-    <t>reason = ISSUER_REJECTED</t>
-  </si>
-  <si>
-    <t>EE_3DS_SCA.REJECTED_INVALID.AUTHORISED</t>
-  </si>
-  <si>
-    <t>reason = INVALID</t>
-  </si>
-  <si>
     <t>EXEMPTION ENGINE TEST DATA</t>
   </si>
   <si>
-    <t>Austria, Finland, Germany, Netherlands, Norway, Sweden, United Kingdom, US</t>
+    <t>https://developer.worldpay.com/docs/wpg/scaexemptionservices/exemptionengine | Note: Please refer Authorisation Flow Magic values only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klarna </t>
+  </si>
+  <si>
+    <t>https://developer.worldpay.com/docs/wpg/apms/klarnakp2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +707,21 @@
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Nova"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -770,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -799,210 +766,6 @@
       <top style="thin">
         <color theme="5"/>
       </top>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="medium">
-        <color theme="5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="medium">
-        <color theme="5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="medium">
-        <color theme="5"/>
-      </right>
-      <top style="medium">
-        <color theme="5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="thin">
-        <color theme="5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="medium">
-        <color theme="5"/>
-      </right>
-      <top style="thin">
-        <color theme="5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="thin">
-        <color theme="5"/>
-      </top>
-      <bottom style="medium">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="thin">
-        <color theme="5"/>
-      </top>
-      <bottom style="medium">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="medium">
-        <color theme="5"/>
-      </right>
-      <top style="thin">
-        <color theme="5"/>
-      </top>
-      <bottom style="medium">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="medium">
-        <color theme="5"/>
-      </top>
-      <bottom style="medium">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top style="medium">
-        <color theme="5"/>
-      </top>
-      <bottom style="medium">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="medium">
-        <color theme="5"/>
-      </right>
-      <top style="medium">
-        <color theme="5"/>
-      </top>
-      <bottom style="medium">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="thin">
-        <color theme="5"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5"/>
-      </left>
-      <right style="medium">
-        <color theme="5"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color theme="5"/>
       </bottom>
@@ -1047,40 +810,47 @@
     </border>
     <border>
       <left style="medium">
-        <color theme="5"/>
+        <color rgb="FFFF0000"/>
       </left>
       <right/>
-      <top/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
       <bottom style="medium">
-        <color theme="5"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
       <bottom style="medium">
-        <color theme="5"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color theme="5"/>
+        <color rgb="FFFF0000"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
       <bottom style="medium">
-        <color theme="5"/>
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1124,40 +894,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1169,15 +915,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1193,47 +930,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1564,26 +1275,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="F3" s="30" t="s">
+      <c r="C3" s="20"/>
+      <c r="F3" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="F4" s="31" t="s">
+      <c r="C4" s="19"/>
+      <c r="F4" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1874,11 +1585,11 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
       <c r="F23" s="12" t="s">
         <v>124</v>
       </c>
@@ -1890,11 +1601,11 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
       <c r="F24" s="12" t="s">
         <v>126</v>
       </c>
@@ -2046,18 +1757,18 @@
       </c>
     </row>
     <row r="33" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
@@ -2149,14 +1860,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2167,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2180,16 +1891,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" spans="2:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -2272,66 +1983,66 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="35"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
@@ -2390,26 +2101,26 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="24"/>
     </row>
     <row r="29" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
@@ -2589,7 +2300,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2602,11 +2313,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="4" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -2636,7 +2347,7 @@
         <v>155</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2705,7 +2416,7 @@
         <v>169</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2758,7 +2469,7 @@
         <v>180</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D19" s="14"/>
     </row>
@@ -2788,7 +2499,7 @@
         <v>169</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2829,222 +2540,63 @@
     </row>
     <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>218</v>
+        <v>201</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D23"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="11"/>
-    <col min="2" max="2" width="51.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="33" style="11" customWidth="1"/>
+    <col min="2" max="2" width="58.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="11" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+    <row r="4" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47"/>
-    </row>
-    <row r="5" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-    </row>
-    <row r="6" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-    </row>
-    <row r="11" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-    </row>
-    <row r="12" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-    </row>
-    <row r="13" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
-    </row>
-    <row r="14" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="42"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="16" t="s">
-        <v>216</v>
-      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>